<commit_message>
updated import ema files
</commit_message>
<xml_diff>
--- a/data/raw/files28/ag-nu-03-07-30-860-f.xlsx
+++ b/data/raw/files28/ag-nu-03-07-30-860-f.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA55"/>
+  <dimension ref="A1:AA54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,149 +360,149 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Date and time</t>
+          <t>Sat, 25 Mar 2023 14:06:08</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>question_context (multipleChoice)</t>
+          <t>Piacevole</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>question1scs (multipleChoice)</t>
+          <t>Totalmente vero...3</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>question_happiness (smiley)</t>
+          <t>80</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>question_dec2 (multipleChoice)</t>
+          <t>Totalmente falso...5</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>question_dec4 (multipleChoice)</t>
+          <t>Totalmente falso...6</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>question5scs (multipleChoice)</t>
+          <t>Totalmente falso...7</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>question3scs (multipleChoice)</t>
+          <t>Totalmente vero...8</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>question_satisfied (smiley)</t>
+          <t>86</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>question8scs (multipleChoice)</t>
+          <t>Moderatamente vero...10</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>question_dec3 (multipleChoice)</t>
+          <t>Totalmente falso...11</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>question4scs (multipleChoice)</t>
+          <t>Moderatamente falso...12</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>question_dec1 (multipleChoice)</t>
+          <t>Moderatamente vero...13</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>question2scs (multipleChoice)</t>
+          <t>Moderatamente falso...14</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>question_nervous (smiley)</t>
+          <t>0...15</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>question6scs (multipleChoice)</t>
+          <t>Moderatamente vero...16</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>question_sad (smiley)</t>
+          <t>0...17</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>question7scs (multipleChoice)</t>
+          <t>Totalmente vero...18</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>question_emotion (multiSmiley)</t>
+          <t>happy</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>yesnoexam (yesno)</t>
+          <t>...20</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>momentary_emotion_yes (multiSmiley)</t>
+          <t>...21</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>exam_preparation (sliderNegPos)</t>
+          <t>...22</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>grade_exp (sliderNeutralPos)</t>
+          <t>...23</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>momentary_emotion_no (multiSmiley)</t>
+          <t>...24</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>emotion_valence_no (smiley)</t>
+          <t>...25</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>real_grade (sliderNeutralPos)</t>
+          <t>...26</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>emotion_valence_yes (smiley)</t>
+          <t>...27</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sat, 25 Mar 2023 14:06:08</t>
+          <t>Sat, 25 Mar 2023 17:26:15</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Piacevole</t>
+          <t>Né spiacevole né piacevole</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -511,34 +511,34 @@
         </is>
       </c>
       <c r="D2">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Totalmente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="I2">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -558,7 +558,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="O2">
@@ -586,7 +586,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sat, 25 Mar 2023 17:26:15</t>
+          <t>Sat, 25 Mar 2023 19:42:29</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -600,21 +600,21 @@
         </is>
       </c>
       <c r="D3">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -623,11 +623,11 @@
         </is>
       </c>
       <c r="I3">
-        <v>88</v>
+        <v>20</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -647,11 +647,11 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
@@ -659,23 +659,23 @@
         </is>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>Totalmente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>angry, happy</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sat, 25 Mar 2023 19:42:29</t>
+          <t>Sat, 25 Mar 2023 21:17:42</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -685,20 +685,20 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Totalmente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="D4">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -712,11 +712,11 @@
         </is>
       </c>
       <c r="I4">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -736,11 +736,11 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="O4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
@@ -748,7 +748,7 @@
         </is>
       </c>
       <c r="Q4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="R4" t="inlineStr">
         <is>
@@ -757,37 +757,37 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>angry, happy</t>
+          <t>happy</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sat, 25 Mar 2023 21:17:42</t>
+          <t>Sat, 01 Apr 2023 11:26:10</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Né spiacevole né piacevole</t>
+          <t>Piacevole</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Totalmente vero</t>
         </is>
       </c>
       <c r="D5">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -801,7 +801,7 @@
         </is>
       </c>
       <c r="I5">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -853,12 +853,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Sat, 01 Apr 2023 11:26:10</t>
+          <t>Sat, 01 Apr 2023 14:59:15</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Piacevole</t>
+          <t>Né spiacevole né piacevole</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -867,16 +867,16 @@
         </is>
       </c>
       <c r="D6">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -890,7 +890,7 @@
         </is>
       </c>
       <c r="I6">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -942,7 +942,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Sat, 01 Apr 2023 14:59:15</t>
+          <t>Sat, 01 Apr 2023 17:10:32</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -952,11 +952,11 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Totalmente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="D7">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -979,7 +979,7 @@
         </is>
       </c>
       <c r="I7">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1003,11 +1003,11 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="O7">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="P7" t="inlineStr">
         <is>
@@ -1015,7 +1015,7 @@
         </is>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="R7" t="inlineStr">
         <is>
@@ -1031,7 +1031,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Sat, 01 Apr 2023 17:10:32</t>
+          <t>Sat, 01 Apr 2023 19:33:46</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1054,7 +1054,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1068,11 +1068,11 @@
         </is>
       </c>
       <c r="I8">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Leggermente falso</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1096,7 +1096,7 @@
         </is>
       </c>
       <c r="O8">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
@@ -1104,7 +1104,7 @@
         </is>
       </c>
       <c r="Q8">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="R8" t="inlineStr">
         <is>
@@ -1113,14 +1113,14 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>stress</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Sat, 01 Apr 2023 19:33:46</t>
+          <t>Sat, 01 Apr 2023 22:48:50</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1134,16 +1134,16 @@
         </is>
       </c>
       <c r="D9">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1157,11 +1157,11 @@
         </is>
       </c>
       <c r="I9">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Leggermente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1181,11 +1181,11 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="O9">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="P9" t="inlineStr">
         <is>
@@ -1193,7 +1193,7 @@
         </is>
       </c>
       <c r="Q9">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="R9" t="inlineStr">
         <is>
@@ -1209,21 +1209,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Sat, 01 Apr 2023 22:48:50</t>
+          <t>Sat, 08 Apr 2023 10:37:00</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Né spiacevole né piacevole</t>
+          <t>Piacevole</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Totalmente vero</t>
         </is>
       </c>
       <c r="D10">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -1246,11 +1246,11 @@
         </is>
       </c>
       <c r="I10">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1260,12 +1260,12 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Totalmente vero</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1274,11 +1274,11 @@
         </is>
       </c>
       <c r="O10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Totalmente vero</t>
         </is>
       </c>
       <c r="Q10">
@@ -1291,14 +1291,14 @@
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>stress</t>
+          <t>happy</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Sat, 08 Apr 2023 10:37:00</t>
+          <t>Sat, 08 Apr 2023 17:08:41</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="D11">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1331,15 +1331,15 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Totalmente vero</t>
         </is>
       </c>
       <c r="I11">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1375,7 +1375,7 @@
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Totalmente vero</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
@@ -1387,12 +1387,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Sat, 08 Apr 2023 17:08:41</t>
+          <t>Sat, 08 Apr 2023 20:26:43</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Piacevole</t>
+          <t>Molto piacevole</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1401,7 +1401,7 @@
         </is>
       </c>
       <c r="D12">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1420,11 +1420,11 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Totalmente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="I12">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1456,7 +1456,7 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Totalmente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="Q12">
@@ -1464,7 +1464,7 @@
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>Totalmente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
@@ -1476,12 +1476,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Sat, 08 Apr 2023 20:26:43</t>
+          <t>Sat, 08 Apr 2023 21:03:46</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Molto piacevole</t>
+          <t>Piacevole</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1532,7 +1532,7 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>Totalmente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -1545,7 +1545,7 @@
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Totalmente vero</t>
         </is>
       </c>
       <c r="Q13">
@@ -1553,7 +1553,7 @@
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Totalmente vero</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
@@ -1565,7 +1565,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Sat, 08 Apr 2023 21:03:46</t>
+          <t>Sat, 15 Apr 2023 10:56:32</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1575,86 +1575,86 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>Moderatamente vero</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>83</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Leggermente vero</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Totalmente falso</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Totalmente falso</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Leggermente vero</t>
+        </is>
+      </c>
+      <c r="I14">
+        <v>66</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Leggermente vero</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Totalmente falso</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Totalmente falso</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Moderatamente vero</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Totalmente falso</t>
+        </is>
+      </c>
+      <c r="O14">
+        <v>34</v>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>Moderatamente vero</t>
+        </is>
+      </c>
+      <c r="Q14">
+        <v>16</v>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
           <t>Totalmente vero</t>
         </is>
       </c>
-      <c r="D14">
-        <v>100</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Totalmente falso</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Totalmente falso</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Totalmente falso</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
-      <c r="I14">
-        <v>100</v>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>Totalmente falso</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>Totalmente falso</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>Totalmente falso</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>Totalmente falso</t>
-        </is>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>Totalmente vero</t>
-        </is>
-      </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>Totalmente vero</t>
-        </is>
-      </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>stress</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Sat, 15 Apr 2023 10:56:32</t>
+          <t>Sat, 15 Apr 2023 14:14:18</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1668,11 +1668,11 @@
         </is>
       </c>
       <c r="D15">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1682,20 +1682,20 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="I15">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1719,7 +1719,7 @@
         </is>
       </c>
       <c r="O15">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="P15" t="inlineStr">
         <is>
@@ -1727,28 +1727,28 @@
         </is>
       </c>
       <c r="Q15">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>Totalmente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>stress</t>
+          <t>happy</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Sat, 15 Apr 2023 14:14:18</t>
+          <t>Sat, 15 Apr 2023 17:29:27</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Piacevole</t>
+          <t>Né spiacevole né piacevole</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1757,7 +1757,7 @@
         </is>
       </c>
       <c r="D16">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1771,7 +1771,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1780,7 +1780,7 @@
         </is>
       </c>
       <c r="I16">
-        <v>74</v>
+        <v>19</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1808,7 +1808,7 @@
         </is>
       </c>
       <c r="O16">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="P16" t="inlineStr">
         <is>
@@ -1816,7 +1816,7 @@
         </is>
       </c>
       <c r="Q16">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R16" t="inlineStr">
         <is>
@@ -1825,14 +1825,14 @@
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>happy, stress</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Sat, 15 Apr 2023 17:29:27</t>
+          <t>Sat, 15 Apr 2023 19:46:03</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1842,25 +1842,25 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Totalmente vero</t>
         </is>
       </c>
       <c r="D17">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1869,11 +1869,11 @@
         </is>
       </c>
       <c r="I17">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1897,7 +1897,7 @@
         </is>
       </c>
       <c r="O17">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="P17" t="inlineStr">
         <is>
@@ -1905,7 +1905,7 @@
         </is>
       </c>
       <c r="Q17">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="R17" t="inlineStr">
         <is>
@@ -1914,14 +1914,14 @@
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>happy, stress</t>
+          <t>happy</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Sat, 15 Apr 2023 19:46:03</t>
+          <t>Sat, 15 Apr 2023 21:09:35</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1931,25 +1931,25 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Totalmente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="D18">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1958,11 +1958,11 @@
         </is>
       </c>
       <c r="I18">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1986,7 +1986,7 @@
         </is>
       </c>
       <c r="O18">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="P18" t="inlineStr">
         <is>
@@ -1994,7 +1994,7 @@
         </is>
       </c>
       <c r="Q18">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="R18" t="inlineStr">
         <is>
@@ -2010,7 +2010,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Sat, 15 Apr 2023 21:09:35</t>
+          <t>Sun, 16 Apr 2023 20:54:46</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2024,16 +2024,16 @@
         </is>
       </c>
       <c r="D19">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Leggermente falso</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -2047,11 +2047,11 @@
         </is>
       </c>
       <c r="I19">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -2075,7 +2075,7 @@
         </is>
       </c>
       <c r="O19">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="P19" t="inlineStr">
         <is>
@@ -2083,23 +2083,42 @@
         </is>
       </c>
       <c r="Q19">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="R19" t="inlineStr">
         <is>
           <t>Moderatamente vero</t>
         </is>
       </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>happy</t>
-        </is>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="V19">
+        <v>29</v>
+      </c>
+      <c r="W19">
+        <v>24</v>
+      </c>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>stress</t>
+        </is>
+      </c>
+      <c r="Y19">
+        <v>27</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Sun, 16 Apr 2023 20:54:46</t>
+          <t>Mon, 17 Apr 2023 20:37:54</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2113,67 +2132,67 @@
         </is>
       </c>
       <c r="D20">
+        <v>23</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Leggermente vero</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Leggermente vero</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Moderatamente falso</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Moderatamente vero</t>
+        </is>
+      </c>
+      <c r="I20">
+        <v>35</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Leggermente vero</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Totalmente falso</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Moderatamente falso</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>Leggermente vero</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Totalmente falso</t>
+        </is>
+      </c>
+      <c r="O20">
+        <v>30</v>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>Moderatamente vero</t>
+        </is>
+      </c>
+      <c r="Q20">
         <v>20</v>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Leggermente falso</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Moderatamente falso</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Totalmente falso</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
-      <c r="I20">
-        <v>31</v>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>Totalmente falso</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>Totalmente falso</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>Totalmente falso</t>
-        </is>
-      </c>
-      <c r="O20">
-        <v>15</v>
-      </c>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
-      <c r="Q20">
-        <v>23</v>
-      </c>
       <c r="R20" t="inlineStr">
         <is>
           <t>Moderatamente vero</t>
@@ -2181,38 +2200,35 @@
       </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="U20" t="inlineStr">
         <is>
+          <t>happy</t>
+        </is>
+      </c>
+      <c r="X20" t="inlineStr">
+        <is>
           <t>-1</t>
         </is>
       </c>
-      <c r="V20">
-        <v>29</v>
-      </c>
-      <c r="W20">
-        <v>24</v>
-      </c>
-      <c r="X20" t="inlineStr">
-        <is>
-          <t>stress</t>
-        </is>
-      </c>
-      <c r="Y20">
-        <v>27</v>
+      <c r="Z20">
+        <v>66</v>
+      </c>
+      <c r="AA20">
+        <v>35</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Mon, 17 Apr 2023 20:37:54</t>
+          <t>Sat, 22 Apr 2023 18:15:17</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Né spiacevole né piacevole</t>
+          <t>Piacevole</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -2221,16 +2237,16 @@
         </is>
       </c>
       <c r="D21">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -2244,11 +2260,11 @@
         </is>
       </c>
       <c r="I21">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -2258,12 +2274,12 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
@@ -2272,47 +2288,31 @@
         </is>
       </c>
       <c r="O21">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Totalmente vero</t>
         </is>
       </c>
       <c r="Q21">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="R21" t="inlineStr">
         <is>
           <t>Moderatamente vero</t>
         </is>
       </c>
-      <c r="T21" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="U21" t="inlineStr">
+      <c r="S21" t="inlineStr">
         <is>
           <t>happy</t>
         </is>
-      </c>
-      <c r="X21" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="Z21">
-        <v>66</v>
-      </c>
-      <c r="AA21">
-        <v>35</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Sat, 22 Apr 2023 18:15:17</t>
+          <t>Sat, 22 Apr 2023 19:59:46</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2326,7 +2326,7 @@
         </is>
       </c>
       <c r="D22">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -2340,16 +2340,16 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="I22">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2377,15 +2377,15 @@
         </is>
       </c>
       <c r="O22">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Totalmente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="Q22">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R22" t="inlineStr">
         <is>
@@ -2401,12 +2401,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Sat, 22 Apr 2023 19:59:46</t>
+          <t>Sat, 22 Apr 2023 21:07:30</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Piacevole</t>
+          <t>Spiacevole</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -2415,16 +2415,16 @@
         </is>
       </c>
       <c r="D23">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -2438,11 +2438,11 @@
         </is>
       </c>
       <c r="I23">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2452,29 +2452,29 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Leggermente falso</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="O23">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Leggermente falso</t>
         </is>
       </c>
       <c r="Q23">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="R23" t="inlineStr">
         <is>
@@ -2483,37 +2483,37 @@
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>sad</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Sat, 22 Apr 2023 21:07:30</t>
+          <t>Sat, 29 Apr 2023 10:37:35</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Spiacevole</t>
+          <t>Né spiacevole né piacevole</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Totalmente vero</t>
         </is>
       </c>
       <c r="D24">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -2523,15 +2523,15 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="I24">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2541,59 +2541,59 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>Leggermente falso</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="O24">
-        <v>84</v>
+        <v>2</v>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Leggermente falso</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="Q24">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Totalmente vero</t>
         </is>
       </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>sad</t>
+          <t>happy</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Sat, 29 Apr 2023 10:37:35</t>
+          <t>Sat, 29 Apr 2023 14:52:51</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Né spiacevole né piacevole</t>
+          <t>Piacevole</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Totalmente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="D25">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -2602,7 +2602,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -2616,7 +2616,7 @@
         </is>
       </c>
       <c r="I25">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2630,7 +2630,7 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
@@ -2644,7 +2644,7 @@
         </is>
       </c>
       <c r="O25">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="P25" t="inlineStr">
         <is>
@@ -2656,7 +2656,7 @@
       </c>
       <c r="R25" t="inlineStr">
         <is>
-          <t>Totalmente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="S25" t="inlineStr">
@@ -2668,12 +2668,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Sat, 29 Apr 2023 14:52:51</t>
+          <t>Sat, 29 Apr 2023 17:44:38</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Piacevole</t>
+          <t>Né spiacevole né piacevole</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -2682,7 +2682,7 @@
         </is>
       </c>
       <c r="D26">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -2691,12 +2691,12 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -2705,7 +2705,7 @@
         </is>
       </c>
       <c r="I26">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2719,7 +2719,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
@@ -2733,7 +2733,7 @@
         </is>
       </c>
       <c r="O26">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="P26" t="inlineStr">
         <is>
@@ -2741,7 +2741,7 @@
         </is>
       </c>
       <c r="Q26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R26" t="inlineStr">
         <is>
@@ -2757,12 +2757,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Sat, 29 Apr 2023 17:44:38</t>
+          <t>Sat, 29 Apr 2023 19:39:45</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Né spiacevole né piacevole</t>
+          <t>Piacevole</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2771,7 +2771,7 @@
         </is>
       </c>
       <c r="D27">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -2780,12 +2780,12 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -2794,7 +2794,7 @@
         </is>
       </c>
       <c r="I27">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2830,7 +2830,7 @@
         </is>
       </c>
       <c r="Q27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R27" t="inlineStr">
         <is>
@@ -2846,21 +2846,21 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Sat, 29 Apr 2023 19:39:45</t>
+          <t>Sat, 29 Apr 2023 21:22:45</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Piacevole</t>
+          <t>Né spiacevole né piacevole</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Totalmente vero</t>
         </is>
       </c>
       <c r="D28">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -2869,7 +2869,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -2879,11 +2879,11 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Totalmente vero</t>
         </is>
       </c>
       <c r="I28">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2935,7 +2935,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Sat, 29 Apr 2023 21:22:45</t>
+          <t>Sat, 06 May 2023 10:26:52</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2945,11 +2945,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Totalmente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="D29">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -2958,7 +2958,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -2968,15 +2968,15 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Totalmente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="I29">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2986,7 +2986,7 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
@@ -2996,11 +2996,11 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="O29">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="P29" t="inlineStr">
         <is>
@@ -3008,7 +3008,7 @@
         </is>
       </c>
       <c r="Q29">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="R29" t="inlineStr">
         <is>
@@ -3024,7 +3024,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Sat, 06 May 2023 10:26:52</t>
+          <t>Sat, 06 May 2023 14:50:39</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -3038,11 +3038,11 @@
         </is>
       </c>
       <c r="D30">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3052,7 +3052,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -3061,35 +3061,35 @@
         </is>
       </c>
       <c r="I30">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
+          <t>Moderatamente falso</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Moderatamente falso</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>Moderatamente vero</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
           <t>Leggermente vero</t>
         </is>
       </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>Totalmente falso</t>
-        </is>
-      </c>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>Leggermente vero</t>
-        </is>
-      </c>
-      <c r="M30" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
       <c r="N30" t="inlineStr">
         <is>
           <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="O30">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="P30" t="inlineStr">
         <is>
@@ -3097,7 +3097,7 @@
         </is>
       </c>
       <c r="Q30">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="R30" t="inlineStr">
         <is>
@@ -3113,12 +3113,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Sat, 06 May 2023 14:50:39</t>
+          <t>Sat, 06 May 2023 17:51:44</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Né spiacevole né piacevole</t>
+          <t>Piacevole</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -3127,7 +3127,7 @@
         </is>
       </c>
       <c r="D31">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -3150,7 +3150,7 @@
         </is>
       </c>
       <c r="I31">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3164,12 +3164,12 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
@@ -3178,15 +3178,15 @@
         </is>
       </c>
       <c r="O31">
+        <v>18</v>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>Moderatamente vero</t>
+        </is>
+      </c>
+      <c r="Q31">
         <v>24</v>
-      </c>
-      <c r="P31" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
-      <c r="Q31">
-        <v>25</v>
       </c>
       <c r="R31" t="inlineStr">
         <is>
@@ -3202,12 +3202,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Sat, 06 May 2023 17:51:44</t>
+          <t>Sat, 06 May 2023 19:56:58</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Piacevole</t>
+          <t>Né spiacevole né piacevole</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -3216,7 +3216,7 @@
         </is>
       </c>
       <c r="D32">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -3230,7 +3230,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -3239,7 +3239,7 @@
         </is>
       </c>
       <c r="I32">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3248,7 +3248,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -3267,7 +3267,7 @@
         </is>
       </c>
       <c r="O32">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P32" t="inlineStr">
         <is>
@@ -3275,7 +3275,7 @@
         </is>
       </c>
       <c r="Q32">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="R32" t="inlineStr">
         <is>
@@ -3291,7 +3291,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Sat, 06 May 2023 19:56:58</t>
+          <t>Sat, 06 May 2023 21:24:14</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3305,7 +3305,7 @@
         </is>
       </c>
       <c r="D33">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -3314,21 +3314,21 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="I33">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3337,7 +3337,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -3356,15 +3356,15 @@
         </is>
       </c>
       <c r="O33">
+        <v>21</v>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>Moderatamente vero</t>
+        </is>
+      </c>
+      <c r="Q33">
         <v>17</v>
-      </c>
-      <c r="P33" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
-      <c r="Q33">
-        <v>29</v>
       </c>
       <c r="R33" t="inlineStr">
         <is>
@@ -3380,7 +3380,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Sat, 06 May 2023 21:24:14</t>
+          <t>Sat, 13 May 2023 10:50:46</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3394,30 +3394,30 @@
         </is>
       </c>
       <c r="D34">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="I34">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
@@ -3445,7 +3445,7 @@
         </is>
       </c>
       <c r="O34">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="P34" t="inlineStr">
         <is>
@@ -3453,7 +3453,7 @@
         </is>
       </c>
       <c r="Q34">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R34" t="inlineStr">
         <is>
@@ -3469,12 +3469,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Sat, 13 May 2023 10:50:46</t>
+          <t>Sat, 13 May 2023 14:29:26</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Né spiacevole né piacevole</t>
+          <t>Piacevole</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -3483,7 +3483,7 @@
         </is>
       </c>
       <c r="D35">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -3492,7 +3492,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -3506,21 +3506,21 @@
         </is>
       </c>
       <c r="I35">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
@@ -3530,11 +3530,11 @@
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="O35">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="P35" t="inlineStr">
         <is>
@@ -3542,7 +3542,7 @@
         </is>
       </c>
       <c r="Q35">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R35" t="inlineStr">
         <is>
@@ -3558,12 +3558,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Sat, 13 May 2023 14:29:26</t>
+          <t>Sat, 13 May 2023 17:26:05</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Piacevole</t>
+          <t>Né spiacevole né piacevole</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -3572,7 +3572,7 @@
         </is>
       </c>
       <c r="D36">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -3581,12 +3581,12 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -3599,7 +3599,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3609,7 +3609,7 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
@@ -3619,11 +3619,11 @@
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="O36">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="P36" t="inlineStr">
         <is>
@@ -3631,7 +3631,7 @@
         </is>
       </c>
       <c r="Q36">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="R36" t="inlineStr">
         <is>
@@ -3647,12 +3647,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Sat, 13 May 2023 17:26:05</t>
+          <t>Sat, 13 May 2023 19:08:10</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Né spiacevole né piacevole</t>
+          <t>Piacevole</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -3661,7 +3661,7 @@
         </is>
       </c>
       <c r="D37">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -3670,12 +3670,12 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -3684,11 +3684,11 @@
         </is>
       </c>
       <c r="I37">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3708,11 +3708,11 @@
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="O37">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="P37" t="inlineStr">
         <is>
@@ -3720,11 +3720,11 @@
         </is>
       </c>
       <c r="Q37">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="R37" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Totalmente vero</t>
         </is>
       </c>
       <c r="S37" t="inlineStr">
@@ -3736,7 +3736,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Sat, 13 May 2023 19:08:10</t>
+          <t>Sat, 13 May 2023 21:21:30</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3750,7 +3750,7 @@
         </is>
       </c>
       <c r="D38">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -3773,7 +3773,7 @@
         </is>
       </c>
       <c r="I38">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -3809,11 +3809,11 @@
         </is>
       </c>
       <c r="Q38">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R38" t="inlineStr">
         <is>
-          <t>Totalmente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="S38" t="inlineStr">
@@ -3825,12 +3825,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Sat, 13 May 2023 21:21:30</t>
+          <t>Sat, 20 May 2023 10:35:22</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Piacevole</t>
+          <t>Né spiacevole né piacevole</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -3839,16 +3839,16 @@
         </is>
       </c>
       <c r="D39">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Leggermente falso</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -3862,11 +3862,11 @@
         </is>
       </c>
       <c r="I39">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3876,7 +3876,7 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
@@ -3886,11 +3886,11 @@
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="O39">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="P39" t="inlineStr">
         <is>
@@ -3898,7 +3898,7 @@
         </is>
       </c>
       <c r="Q39">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="R39" t="inlineStr">
         <is>
@@ -3914,12 +3914,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Sat, 20 May 2023 10:35:22</t>
+          <t>Sat, 20 May 2023 19:27:05</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Né spiacevole né piacevole</t>
+          <t>Molto piacevole</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -3928,21 +3928,21 @@
         </is>
       </c>
       <c r="D40">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente vero</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Leggermente falso</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -3951,16 +3951,16 @@
         </is>
       </c>
       <c r="I40">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente vero</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3975,23 +3975,23 @@
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="O40">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="Q40">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="R40" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="S40" t="inlineStr">
@@ -4003,12 +4003,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Sat, 20 May 2023 19:27:05</t>
+          <t>Sat, 20 May 2023 21:32:19</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Molto piacevole</t>
+          <t>Né spiacevole né piacevole</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -4017,34 +4017,34 @@
         </is>
       </c>
       <c r="D41">
+        <v>62</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Leggermente vero</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Moderatamente falso</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Totalmente falso</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Moderatamente vero</t>
+        </is>
+      </c>
+      <c r="I41">
         <v>83</v>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>Totalmente vero</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>Leggermente vero</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
-      <c r="I41">
-        <v>85</v>
-      </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Totalmente vero</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -4064,23 +4064,23 @@
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="O41">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="Q41">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="R41" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="S41" t="inlineStr">
@@ -4092,7 +4092,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Sat, 20 May 2023 21:32:19</t>
+          <t>Sun, 21 May 2023 20:04:51</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -4106,11 +4106,11 @@
         </is>
       </c>
       <c r="D42">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Leggermente falso</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -4120,7 +4120,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -4129,16 +4129,16 @@
         </is>
       </c>
       <c r="I42">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -4153,11 +4153,11 @@
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="O42">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="P42" t="inlineStr">
         <is>
@@ -4165,28 +4165,44 @@
         </is>
       </c>
       <c r="Q42">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="R42" t="inlineStr">
         <is>
           <t>Moderatamente vero</t>
         </is>
       </c>
-      <c r="S42" t="inlineStr">
+      <c r="T42" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="U42" t="inlineStr">
         <is>
           <t>happy</t>
         </is>
+      </c>
+      <c r="X42" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="Z42">
+        <v>63</v>
+      </c>
+      <c r="AA42">
+        <v>59</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Sun, 21 May 2023 20:04:51</t>
+          <t>Mon, 22 May 2023 20:56:32</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Né spiacevole né piacevole</t>
+          <t>Piacevole</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -4195,11 +4211,11 @@
         </is>
       </c>
       <c r="D43">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Leggermente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -4209,7 +4225,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -4218,11 +4234,11 @@
         </is>
       </c>
       <c r="I43">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -4232,7 +4248,7 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
@@ -4242,11 +4258,11 @@
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="O43">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="P43" t="inlineStr">
         <is>
@@ -4254,7 +4270,7 @@
         </is>
       </c>
       <c r="Q43">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="R43" t="inlineStr">
         <is>
@@ -4277,16 +4293,16 @@
         </is>
       </c>
       <c r="Z43">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="AA43">
-        <v>59</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Mon, 22 May 2023 20:56:32</t>
+          <t>Tue, 23 May 2023 20:33:37</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -4300,16 +4316,16 @@
         </is>
       </c>
       <c r="D44">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -4323,7 +4339,7 @@
         </is>
       </c>
       <c r="I44">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4351,7 +4367,7 @@
         </is>
       </c>
       <c r="O44">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="P44" t="inlineStr">
         <is>
@@ -4359,7 +4375,7 @@
         </is>
       </c>
       <c r="Q44">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="R44" t="inlineStr">
         <is>
@@ -4382,34 +4398,34 @@
         </is>
       </c>
       <c r="Z44">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="AA44">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Tue, 23 May 2023 20:33:37</t>
+          <t>Wed, 24 May 2023 20:14:47</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Piacevole</t>
+          <t>Spiacevole</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Leggermente falso</t>
         </is>
       </c>
       <c r="D45">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -4419,20 +4435,20 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="I45">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -4442,33 +4458,33 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="O45">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Leggermente falso</t>
         </is>
       </c>
       <c r="Q45">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="R45" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="T45" t="inlineStr">
@@ -4478,7 +4494,7 @@
       </c>
       <c r="U45" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>angry</t>
         </is>
       </c>
       <c r="X45" t="inlineStr">
@@ -4487,93 +4503,93 @@
         </is>
       </c>
       <c r="Z45">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AA45">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Wed, 24 May 2023 20:14:47</t>
+          <t>Thu, 25 May 2023 20:51:09</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Spiacevole</t>
+          <t>Piacevole</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
+          <t>Totalmente vero</t>
+        </is>
+      </c>
+      <c r="D46">
+        <v>100</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Leggermente vero</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Moderatamente falso</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Leggermente vero</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Moderatamente vero</t>
+        </is>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Leggermente vero</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>Totalmente falso</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Totalmente falso</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>Totalmente vero</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
           <t>Leggermente falso</t>
         </is>
       </c>
-      <c r="D46">
-        <v>16</v>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>Leggermente vero</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>Leggermente vero</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>Leggermente vero</t>
-        </is>
-      </c>
-      <c r="I46">
-        <v>5</v>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>Totalmente falso</t>
-        </is>
-      </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>Moderatamente falso</t>
-        </is>
-      </c>
-      <c r="N46" t="inlineStr">
-        <is>
-          <t>Leggermente vero</t>
-        </is>
-      </c>
       <c r="O46">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Leggermente falso</t>
+          <t>Totalmente vero</t>
         </is>
       </c>
       <c r="Q46">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="R46" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="T46" t="inlineStr">
@@ -4583,7 +4599,7 @@
       </c>
       <c r="U46" t="inlineStr">
         <is>
-          <t>angry</t>
+          <t>happy</t>
         </is>
       </c>
       <c r="X46" t="inlineStr">
@@ -4592,16 +4608,16 @@
         </is>
       </c>
       <c r="Z46">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="AA46">
-        <v>77</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Thu, 25 May 2023 20:51:09</t>
+          <t>Sat, 27 May 2023 10:10:27</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -4611,38 +4627,38 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Totalmente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="D47">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
+          <t>Moderatamente falso</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Moderatamente falso</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Moderatamente falso</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
           <t>Leggermente vero</t>
         </is>
       </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>Moderatamente falso</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>Leggermente vero</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
       <c r="I47">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -4652,61 +4668,45 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>Totalmente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>Leggermente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="O47">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Totalmente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="Q47">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="R47" t="inlineStr">
         <is>
           <t>Moderatamente vero</t>
         </is>
       </c>
-      <c r="T47" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="U47" t="inlineStr">
-        <is>
-          <t>happy</t>
-        </is>
-      </c>
-      <c r="X47" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="Z47">
-        <v>85</v>
-      </c>
-      <c r="AA47">
-        <v>53</v>
+      <c r="S47" t="inlineStr">
+        <is>
+          <t>happy, stress</t>
+        </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Sat, 27 May 2023 10:10:27</t>
+          <t>Sat, 27 May 2023 14:10:46</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4720,7 +4720,7 @@
         </is>
       </c>
       <c r="D48">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -4729,12 +4729,12 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -4743,11 +4743,11 @@
         </is>
       </c>
       <c r="I48">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Leggermente falso</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -4757,7 +4757,7 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
@@ -4771,7 +4771,7 @@
         </is>
       </c>
       <c r="O48">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="P48" t="inlineStr">
         <is>
@@ -4779,7 +4779,7 @@
         </is>
       </c>
       <c r="Q48">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="R48" t="inlineStr">
         <is>
@@ -4788,14 +4788,14 @@
       </c>
       <c r="S48" t="inlineStr">
         <is>
-          <t>happy, stress</t>
+          <t>happy</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Sat, 27 May 2023 14:10:46</t>
+          <t>Sat, 27 May 2023 19:18:28</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4809,16 +4809,16 @@
         </is>
       </c>
       <c r="D49">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -4828,15 +4828,15 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="I49">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Leggermente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -4856,11 +4856,11 @@
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="O49">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="P49" t="inlineStr">
         <is>
@@ -4868,7 +4868,7 @@
         </is>
       </c>
       <c r="Q49">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="R49" t="inlineStr">
         <is>
@@ -4884,40 +4884,40 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Sat, 27 May 2023 19:18:28</t>
+          <t>Sat, 27 May 2023 21:11:59</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Piacevole</t>
+          <t>Spiacevole</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="D50">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Leggermente falso</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente vero</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Totalmente vero</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="I50">
@@ -4925,35 +4925,35 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Leggermente falso</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Leggermente falso</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="O50">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Leggermente falso</t>
         </is>
       </c>
       <c r="Q50">
@@ -4961,7 +4961,7 @@
       </c>
       <c r="R50" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="S50" t="inlineStr">
@@ -4973,63 +4973,63 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Sat, 27 May 2023 21:11:59</t>
+          <t>Sat, 03 Jun 2023 10:04:43</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Spiacevole</t>
+          <t>Né spiacevole né piacevole</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
+          <t>Moderatamente vero</t>
+        </is>
+      </c>
+      <c r="D51">
+        <v>26</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Leggermente falso</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
           <t>Leggermente vero</t>
         </is>
       </c>
-      <c r="D51">
-        <v>100</v>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>Leggermente falso</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>Totalmente vero</t>
-        </is>
-      </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Totalmente vero</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="I51">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Leggermente falso</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
+          <t>Totalmente falso</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
           <t>Leggermente vero</t>
         </is>
       </c>
-      <c r="L51" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>Leggermente falso</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
@@ -5038,36 +5038,36 @@
         </is>
       </c>
       <c r="O51">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Leggermente falso</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="Q51">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="R51" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="S51" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>stress, happy</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Sat, 03 Jun 2023 10:04:43</t>
+          <t>Sat, 03 Jun 2023 14:38:07</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Né spiacevole né piacevole</t>
+          <t>Piacevole</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -5076,7 +5076,7 @@
         </is>
       </c>
       <c r="D52">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -5085,57 +5085,57 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
+          <t>Totalmente falso</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Moderatamente falso</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
           <t>Leggermente vero</t>
         </is>
       </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>Totalmente falso</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
       <c r="I52">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
+          <t>Moderatamente vero</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>Totalmente falso</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
           <t>Leggermente vero</t>
         </is>
       </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>Totalmente falso</t>
-        </is>
-      </c>
-      <c r="L52" t="inlineStr">
+      <c r="M52" t="inlineStr">
         <is>
           <t>Leggermente vero</t>
         </is>
       </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="O52">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="Q52">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="R52" t="inlineStr">
         <is>
@@ -5144,14 +5144,14 @@
       </c>
       <c r="S52" t="inlineStr">
         <is>
-          <t>stress, happy</t>
+          <t>happy, stress</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Sat, 03 Jun 2023 14:38:07</t>
+          <t>Sat, 03 Jun 2023 17:44:36</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -5165,11 +5165,11 @@
         </is>
       </c>
       <c r="D53">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Leggermente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -5179,20 +5179,20 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="I53">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -5202,12 +5202,12 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
@@ -5216,15 +5216,15 @@
         </is>
       </c>
       <c r="O53">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Leggermente vero</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="Q53">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="R53" t="inlineStr">
         <is>
@@ -5240,12 +5240,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Sat, 03 Jun 2023 17:44:36</t>
+          <t>Sat, 03 Jun 2023 19:44:30</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Piacevole</t>
+          <t>Né spiacevole né piacevole</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -5254,162 +5254,73 @@
         </is>
       </c>
       <c r="D54">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Totalmente falso</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Moderatamente vero</t>
+          <t>Leggermente falso</t>
         </is>
       </c>
       <c r="I54">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Moderatamente falso</t>
+          <t>Leggermente vero</t>
         </is>
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>Totalmente falso</t>
+          <t>Moderatamente falso</t>
         </is>
       </c>
       <c r="O54">
+        <v>22</v>
+      </c>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>Moderatamente vero</t>
+        </is>
+      </c>
+      <c r="Q54">
         <v>20</v>
       </c>
-      <c r="P54" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
-      <c r="Q54">
-        <v>15</v>
-      </c>
       <c r="R54" t="inlineStr">
         <is>
           <t>Moderatamente vero</t>
         </is>
       </c>
       <c r="S54" t="inlineStr">
-        <is>
-          <t>happy, stress</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>Sat, 03 Jun 2023 19:44:30</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Né spiacevole né piacevole</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
-      <c r="D55">
-        <v>18</v>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>Totalmente falso</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>Leggermente vero</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>Leggermente vero</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>Leggermente falso</t>
-        </is>
-      </c>
-      <c r="I55">
-        <v>21</v>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>Moderatamente falso</t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>Moderatamente falso</t>
-        </is>
-      </c>
-      <c r="L55" t="inlineStr">
-        <is>
-          <t>Leggermente vero</t>
-        </is>
-      </c>
-      <c r="M55" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
-      <c r="N55" t="inlineStr">
-        <is>
-          <t>Moderatamente falso</t>
-        </is>
-      </c>
-      <c r="O55">
-        <v>22</v>
-      </c>
-      <c r="P55" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
-      <c r="Q55">
-        <v>20</v>
-      </c>
-      <c r="R55" t="inlineStr">
-        <is>
-          <t>Moderatamente vero</t>
-        </is>
-      </c>
-      <c r="S55" t="inlineStr">
         <is>
           <t>happy, stress</t>
         </is>

</xml_diff>